<commit_message>
Fix tonen 0 waardes
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_HarmonizeV2.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_HarmonizeV2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927C9E68-3400-A74A-8093-9238D7A50D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20ADB4B-973D-ED4A-9AC2-5E6012F8D3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -439,9 +439,6 @@
     <t>vullingnr</t>
   </si>
   <si>
-    <t>["VULLING", "VULLINGNO"]</t>
-  </si>
-  <si>
     <t>bioturbatie</t>
   </si>
   <si>
@@ -1943,6 +1940,9 @@
   </si>
   <si>
     <t>["METAAL", "ARTF_MET", "SPIJKER.*"]</t>
+  </si>
+  <si>
+    <t>["VULLING", "VULLINGNO", "MUUR"]</t>
   </si>
 </sst>
 </file>
@@ -2399,7 +2399,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2484,10 +2484,10 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
+        <v>566</v>
+      </c>
+      <c r="C9" t="s">
         <v>567</v>
-      </c>
-      <c r="C9" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2495,10 +2495,10 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C10" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2548,7 +2548,7 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -2565,7 +2565,7 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2582,7 +2582,7 @@
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2599,7 +2599,7 @@
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -2616,7 +2616,7 @@
         <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -2627,13 +2627,13 @@
         <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -2650,7 +2650,7 @@
         <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -2661,13 +2661,13 @@
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -2675,7 +2675,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
@@ -2684,7 +2684,7 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -2692,16 +2692,16 @@
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C23" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D23" t="s">
         <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -2709,16 +2709,16 @@
         <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C24" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D24" t="s">
         <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -2735,7 +2735,7 @@
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2752,10 +2752,10 @@
         <v>20</v>
       </c>
       <c r="F26" t="s">
+        <v>603</v>
+      </c>
+      <c r="G26" t="s">
         <v>604</v>
-      </c>
-      <c r="G26" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -2772,7 +2772,7 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
   </sheetData>
@@ -2804,7 +2804,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2812,10 +2812,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" t="s">
         <v>273</v>
-      </c>
-      <c r="C2" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2823,10 +2823,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2834,10 +2834,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C4" t="s">
         <v>276</v>
-      </c>
-      <c r="C4" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2845,10 +2845,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2856,10 +2856,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2867,10 +2867,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C7" t="s">
         <v>280</v>
-      </c>
-      <c r="C7" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2878,10 +2878,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" t="s">
         <v>282</v>
-      </c>
-      <c r="C8" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2889,10 +2889,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C9" t="s">
         <v>284</v>
-      </c>
-      <c r="C9" t="s">
-        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -2923,7 +2923,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2931,10 +2931,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C2" t="s">
         <v>286</v>
-      </c>
-      <c r="C2" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2942,10 +2942,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C3" t="s">
         <v>288</v>
-      </c>
-      <c r="C3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2953,10 +2953,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C4" t="s">
         <v>290</v>
-      </c>
-      <c r="C4" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2964,10 +2964,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" t="s">
         <v>292</v>
-      </c>
-      <c r="C5" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2975,10 +2975,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C6" t="s">
         <v>294</v>
-      </c>
-      <c r="C6" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2986,10 +2986,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C7" t="s">
         <v>296</v>
-      </c>
-      <c r="C7" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2997,10 +2997,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>297</v>
+      </c>
+      <c r="C8" t="s">
         <v>298</v>
-      </c>
-      <c r="C8" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3008,10 +3008,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C9" t="s">
         <v>300</v>
-      </c>
-      <c r="C9" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3019,10 +3019,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>301</v>
+      </c>
+      <c r="C10" t="s">
         <v>302</v>
-      </c>
-      <c r="C10" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3030,10 +3030,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>303</v>
+      </c>
+      <c r="C11" t="s">
         <v>304</v>
-      </c>
-      <c r="C11" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3041,10 +3041,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3052,10 +3052,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>306</v>
+      </c>
+      <c r="C13" t="s">
         <v>307</v>
-      </c>
-      <c r="C13" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3063,10 +3063,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C14" t="s">
         <v>309</v>
-      </c>
-      <c r="C14" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3074,10 +3074,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>310</v>
+      </c>
+      <c r="C15" t="s">
         <v>311</v>
-      </c>
-      <c r="C15" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3085,10 +3085,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C16" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3096,10 +3096,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3107,10 +3107,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>314</v>
+      </c>
+      <c r="C18" t="s">
         <v>315</v>
-      </c>
-      <c r="C18" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3118,10 +3118,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>316</v>
+      </c>
+      <c r="C19" t="s">
         <v>317</v>
-      </c>
-      <c r="C19" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3129,10 +3129,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>318</v>
+      </c>
+      <c r="C20" t="s">
         <v>319</v>
-      </c>
-      <c r="C20" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3140,10 +3140,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>320</v>
+      </c>
+      <c r="C21" t="s">
         <v>321</v>
-      </c>
-      <c r="C21" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3151,10 +3151,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>322</v>
+      </c>
+      <c r="C22" t="s">
         <v>323</v>
-      </c>
-      <c r="C22" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3162,10 +3162,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>324</v>
+      </c>
+      <c r="C23" t="s">
         <v>325</v>
-      </c>
-      <c r="C23" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3173,10 +3173,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>326</v>
+      </c>
+      <c r="C24" t="s">
         <v>327</v>
-      </c>
-      <c r="C24" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3184,10 +3184,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>328</v>
+      </c>
+      <c r="C25" t="s">
         <v>329</v>
-      </c>
-      <c r="C25" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3198,7 +3198,7 @@
         <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -3220,7 +3220,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>45</v>
@@ -3229,7 +3229,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3253,7 +3253,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3261,10 +3261,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3272,10 +3272,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C3" t="s">
         <v>333</v>
-      </c>
-      <c r="C3" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3283,10 +3283,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C4" t="s">
         <v>335</v>
-      </c>
-      <c r="C4" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3294,10 +3294,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C5" t="s">
         <v>337</v>
-      </c>
-      <c r="C5" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3305,10 +3305,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3316,10 +3316,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3327,10 +3327,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>340</v>
+      </c>
+      <c r="C8" t="s">
         <v>341</v>
-      </c>
-      <c r="C8" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3338,10 +3338,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>342</v>
+      </c>
+      <c r="C9" t="s">
         <v>343</v>
-      </c>
-      <c r="C9" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3349,10 +3349,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>344</v>
+      </c>
+      <c r="C10" t="s">
         <v>345</v>
-      </c>
-      <c r="C10" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3360,10 +3360,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>346</v>
+      </c>
+      <c r="C11" t="s">
         <v>347</v>
-      </c>
-      <c r="C11" t="s">
-        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -3387,7 +3387,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3413,7 +3413,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3421,10 +3421,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C2" t="s">
         <v>349</v>
-      </c>
-      <c r="C2" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3432,10 +3432,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C3" t="s">
         <v>351</v>
-      </c>
-      <c r="C3" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3443,10 +3443,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3454,10 +3454,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>353</v>
+      </c>
+      <c r="C5" t="s">
         <v>354</v>
-      </c>
-      <c r="C5" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3465,10 +3465,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>355</v>
+      </c>
+      <c r="C6" t="s">
         <v>356</v>
-      </c>
-      <c r="C6" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3476,10 +3476,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>357</v>
+      </c>
+      <c r="C7" t="s">
         <v>358</v>
-      </c>
-      <c r="C7" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3487,10 +3487,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>359</v>
+      </c>
+      <c r="C8" t="s">
         <v>360</v>
-      </c>
-      <c r="C8" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3498,10 +3498,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>361</v>
+      </c>
+      <c r="C9" t="s">
         <v>362</v>
-      </c>
-      <c r="C9" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3509,10 +3509,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>363</v>
+      </c>
+      <c r="C10" t="s">
         <v>364</v>
-      </c>
-      <c r="C10" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3520,10 +3520,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>365</v>
+      </c>
+      <c r="C11" t="s">
         <v>366</v>
-      </c>
-      <c r="C11" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3531,10 +3531,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>367</v>
+      </c>
+      <c r="C12" t="s">
         <v>368</v>
-      </c>
-      <c r="C12" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3542,10 +3542,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>369</v>
+      </c>
+      <c r="C13" t="s">
         <v>370</v>
-      </c>
-      <c r="C13" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3553,10 +3553,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3564,10 +3564,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>371</v>
+      </c>
+      <c r="C15" t="s">
         <v>372</v>
-      </c>
-      <c r="C15" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3575,10 +3575,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>373</v>
+      </c>
+      <c r="C16" t="s">
         <v>374</v>
-      </c>
-      <c r="C16" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3586,10 +3586,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>375</v>
+      </c>
+      <c r="C17" t="s">
         <v>376</v>
-      </c>
-      <c r="C17" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3597,10 +3597,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>377</v>
+      </c>
+      <c r="C18" t="s">
         <v>378</v>
-      </c>
-      <c r="C18" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3608,10 +3608,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3619,10 +3619,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>379</v>
+      </c>
+      <c r="C20" t="s">
         <v>380</v>
-      </c>
-      <c r="C20" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3630,10 +3630,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>381</v>
+      </c>
+      <c r="C21" t="s">
         <v>382</v>
-      </c>
-      <c r="C21" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3641,10 +3641,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C22" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3652,10 +3652,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>384</v>
+      </c>
+      <c r="C23" t="s">
         <v>385</v>
-      </c>
-      <c r="C23" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3663,10 +3663,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>386</v>
+      </c>
+      <c r="C24" t="s">
         <v>387</v>
-      </c>
-      <c r="C24" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3674,10 +3674,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>388</v>
+      </c>
+      <c r="C25" t="s">
         <v>389</v>
-      </c>
-      <c r="C25" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3685,10 +3685,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>390</v>
+      </c>
+      <c r="C26" t="s">
         <v>391</v>
-      </c>
-      <c r="C26" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3696,10 +3696,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
+        <v>392</v>
+      </c>
+      <c r="C27" t="s">
         <v>393</v>
-      </c>
-      <c r="C27" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3707,10 +3707,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>394</v>
+      </c>
+      <c r="C28" t="s">
         <v>395</v>
-      </c>
-      <c r="C28" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3718,10 +3718,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
+        <v>396</v>
+      </c>
+      <c r="C29" t="s">
         <v>397</v>
-      </c>
-      <c r="C29" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3729,10 +3729,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
+        <v>398</v>
+      </c>
+      <c r="C30" t="s">
         <v>399</v>
-      </c>
-      <c r="C30" t="s">
-        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -3762,7 +3762,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3770,10 +3770,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3781,10 +3781,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C3" t="s">
         <v>402</v>
-      </c>
-      <c r="C3" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3792,10 +3792,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3803,10 +3803,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>404</v>
+      </c>
+      <c r="C5" t="s">
         <v>405</v>
-      </c>
-      <c r="C5" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3814,10 +3814,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>406</v>
+      </c>
+      <c r="C6" t="s">
         <v>407</v>
-      </c>
-      <c r="C6" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3825,10 +3825,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>408</v>
+      </c>
+      <c r="C7" t="s">
         <v>409</v>
-      </c>
-      <c r="C7" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3836,10 +3836,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3847,10 +3847,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3858,10 +3858,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3869,10 +3869,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C11" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3880,10 +3880,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>414</v>
+      </c>
+      <c r="C12" t="s">
         <v>415</v>
-      </c>
-      <c r="C12" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3891,10 +3891,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>416</v>
+      </c>
+      <c r="C13" t="s">
         <v>417</v>
-      </c>
-      <c r="C13" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3902,10 +3902,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3913,10 +3913,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>419</v>
+      </c>
+      <c r="C15" t="s">
         <v>420</v>
-      </c>
-      <c r="C15" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3924,10 +3924,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C16" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3935,10 +3935,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>215</v>
+      </c>
+      <c r="C17" t="s">
         <v>216</v>
-      </c>
-      <c r="C17" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3946,10 +3946,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3957,10 +3957,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C19" t="s">
         <v>423</v>
-      </c>
-      <c r="C19" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3968,10 +3968,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>424</v>
+      </c>
+      <c r="C20" t="s">
         <v>425</v>
-      </c>
-      <c r="C20" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3979,10 +3979,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C21" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3990,10 +3990,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>283</v>
+      </c>
+      <c r="C22" t="s">
         <v>284</v>
-      </c>
-      <c r="C22" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -4001,10 +4001,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>427</v>
+      </c>
+      <c r="C23" t="s">
         <v>428</v>
-      </c>
-      <c r="C23" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -4012,10 +4012,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>429</v>
+      </c>
+      <c r="C24" t="s">
         <v>430</v>
-      </c>
-      <c r="C24" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -4023,10 +4023,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>431</v>
+      </c>
+      <c r="C25" t="s">
         <v>432</v>
-      </c>
-      <c r="C25" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -4034,10 +4034,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>433</v>
+      </c>
+      <c r="C26" t="s">
         <v>434</v>
-      </c>
-      <c r="C26" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -4045,10 +4045,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>238</v>
+      </c>
+      <c r="C27" t="s">
         <v>239</v>
-      </c>
-      <c r="C27" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -4059,7 +4059,7 @@
         <v>74</v>
       </c>
       <c r="C28" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -4087,7 +4087,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4095,10 +4095,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4106,10 +4106,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4117,10 +4117,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>436</v>
+      </c>
+      <c r="C4" t="s">
         <v>437</v>
-      </c>
-      <c r="C4" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4128,10 +4128,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C5" t="s">
         <v>439</v>
-      </c>
-      <c r="C5" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4139,10 +4139,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6" t="s">
         <v>201</v>
-      </c>
-      <c r="C6" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4150,10 +4150,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>440</v>
+      </c>
+      <c r="C7" t="s">
         <v>441</v>
-      </c>
-      <c r="C7" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4161,10 +4161,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4172,10 +4172,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>442</v>
+      </c>
+      <c r="C9" t="s">
         <v>443</v>
-      </c>
-      <c r="C9" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4183,10 +4183,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4194,10 +4194,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4205,10 +4205,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>446</v>
+      </c>
+      <c r="C12" t="s">
         <v>447</v>
-      </c>
-      <c r="C12" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4216,10 +4216,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C13" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4227,10 +4227,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>449</v>
+      </c>
+      <c r="C14" t="s">
         <v>450</v>
-      </c>
-      <c r="C14" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4238,10 +4238,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>451</v>
+      </c>
+      <c r="C15" t="s">
         <v>452</v>
-      </c>
-      <c r="C15" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4249,10 +4249,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>453</v>
+      </c>
+      <c r="C16" t="s">
         <v>454</v>
-      </c>
-      <c r="C16" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -4260,10 +4260,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>455</v>
+      </c>
+      <c r="C17" t="s">
         <v>456</v>
-      </c>
-      <c r="C17" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -4271,10 +4271,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>457</v>
+      </c>
+      <c r="C18" t="s">
         <v>458</v>
-      </c>
-      <c r="C18" t="s">
-        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -4298,7 +4298,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4306,10 +4306,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>459</v>
+      </c>
+      <c r="C2" t="s">
         <v>460</v>
-      </c>
-      <c r="C2" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4317,10 +4317,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4328,10 +4328,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4339,10 +4339,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" t="s">
         <v>276</v>
-      </c>
-      <c r="C5" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4350,10 +4350,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>462</v>
+      </c>
+      <c r="C6" t="s">
         <v>463</v>
-      </c>
-      <c r="C6" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4361,10 +4361,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>464</v>
+      </c>
+      <c r="C7" t="s">
         <v>465</v>
-      </c>
-      <c r="C7" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4372,10 +4372,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4383,10 +4383,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4394,10 +4394,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>468</v>
+      </c>
+      <c r="C10" t="s">
         <v>469</v>
-      </c>
-      <c r="C10" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4405,10 +4405,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>470</v>
+      </c>
+      <c r="C11" t="s">
         <v>471</v>
-      </c>
-      <c r="C11" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4416,10 +4416,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>472</v>
+      </c>
+      <c r="C12" t="s">
         <v>473</v>
-      </c>
-      <c r="C12" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4427,10 +4427,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>474</v>
+      </c>
+      <c r="C13" t="s">
         <v>475</v>
-      </c>
-      <c r="C13" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4438,10 +4438,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C14" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4449,10 +4449,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>477</v>
+      </c>
+      <c r="C15" t="s">
         <v>478</v>
-      </c>
-      <c r="C15" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4460,10 +4460,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>479</v>
+      </c>
+      <c r="C16" t="s">
         <v>480</v>
-      </c>
-      <c r="C16" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -4471,10 +4471,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>481</v>
+      </c>
+      <c r="C17" t="s">
         <v>482</v>
-      </c>
-      <c r="C17" t="s">
-        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -4498,7 +4498,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4506,10 +4506,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4517,10 +4517,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4528,10 +4528,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C4" t="s">
         <v>358</v>
-      </c>
-      <c r="C4" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4539,10 +4539,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4550,10 +4550,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4561,10 +4561,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>487</v>
+      </c>
+      <c r="C7" t="s">
         <v>488</v>
-      </c>
-      <c r="C7" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4572,10 +4572,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C8" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4583,10 +4583,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4594,10 +4594,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>491</v>
+      </c>
+      <c r="C10" t="s">
         <v>492</v>
-      </c>
-      <c r="C10" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4605,10 +4605,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C11" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4616,10 +4616,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4627,10 +4627,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>495</v>
+      </c>
+      <c r="C13" t="s">
         <v>496</v>
-      </c>
-      <c r="C13" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4638,10 +4638,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>497</v>
+      </c>
+      <c r="C14" t="s">
         <v>498</v>
-      </c>
-      <c r="C14" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4649,10 +4649,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>499</v>
+      </c>
+      <c r="C15" t="s">
         <v>500</v>
-      </c>
-      <c r="C15" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4660,10 +4660,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>501</v>
+      </c>
+      <c r="C16" t="s">
         <v>502</v>
-      </c>
-      <c r="C16" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -4671,10 +4671,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C17" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -4682,10 +4682,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C18" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -4693,10 +4693,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>504</v>
+      </c>
+      <c r="C19" t="s">
         <v>505</v>
-      </c>
-      <c r="C19" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -4704,10 +4704,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>506</v>
+      </c>
+      <c r="C20" t="s">
         <v>507</v>
-      </c>
-      <c r="C20" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -4715,10 +4715,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C21" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -4726,10 +4726,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>509</v>
+      </c>
+      <c r="C22" t="s">
         <v>510</v>
-      </c>
-      <c r="C22" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -4737,10 +4737,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>511</v>
+      </c>
+      <c r="C23" t="s">
         <v>512</v>
-      </c>
-      <c r="C23" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -4748,10 +4748,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>238</v>
+      </c>
+      <c r="C24" t="s">
         <v>239</v>
-      </c>
-      <c r="C24" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -4762,7 +4762,7 @@
         <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -4770,10 +4770,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>513</v>
+      </c>
+      <c r="C26" t="s">
         <v>514</v>
-      </c>
-      <c r="C26" t="s">
-        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -4883,7 +4883,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4891,10 +4891,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>515</v>
+      </c>
+      <c r="C2" t="s">
         <v>516</v>
-      </c>
-      <c r="C2" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4902,10 +4902,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4913,10 +4913,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>518</v>
+      </c>
+      <c r="C4" t="s">
         <v>519</v>
-      </c>
-      <c r="C4" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4924,10 +4924,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>520</v>
+      </c>
+      <c r="C5" t="s">
         <v>521</v>
-      </c>
-      <c r="C5" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4935,10 +4935,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4946,10 +4946,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C7" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4957,10 +4957,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>523</v>
+      </c>
+      <c r="C8" t="s">
         <v>524</v>
-      </c>
-      <c r="C8" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4968,10 +4968,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4979,10 +4979,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>340</v>
+      </c>
+      <c r="C10" t="s">
         <v>341</v>
-      </c>
-      <c r="C10" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4990,10 +4990,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>526</v>
+      </c>
+      <c r="C11" t="s">
         <v>527</v>
-      </c>
-      <c r="C11" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -5001,10 +5001,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>528</v>
+      </c>
+      <c r="C12" t="s">
         <v>529</v>
-      </c>
-      <c r="C12" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -5012,10 +5012,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>530</v>
+      </c>
+      <c r="C13" t="s">
         <v>531</v>
-      </c>
-      <c r="C13" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -5023,10 +5023,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>532</v>
+      </c>
+      <c r="C14" t="s">
         <v>533</v>
-      </c>
-      <c r="C14" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -5034,10 +5034,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>534</v>
+      </c>
+      <c r="C15" t="s">
         <v>535</v>
-      </c>
-      <c r="C15" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -5045,10 +5045,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>238</v>
+      </c>
+      <c r="C16" t="s">
         <v>239</v>
-      </c>
-      <c r="C16" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -5056,10 +5056,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>536</v>
+      </c>
+      <c r="C17" t="s">
         <v>537</v>
-      </c>
-      <c r="C17" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -5067,10 +5067,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>538</v>
+      </c>
+      <c r="C18" t="s">
         <v>539</v>
-      </c>
-      <c r="C18" t="s">
-        <v>540</v>
       </c>
     </row>
   </sheetData>
@@ -5100,31 +5100,31 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>568</v>
+      </c>
+      <c r="C2" t="s">
         <v>569</v>
-      </c>
-      <c r="C2" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>571</v>
+      </c>
+      <c r="C4" t="s">
         <v>572</v>
-      </c>
-      <c r="C4" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
@@ -5140,7 +5140,7 @@
         <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
@@ -5148,7 +5148,7 @@
         <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
@@ -5156,15 +5156,15 @@
         <v>108</v>
       </c>
       <c r="C8" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>576</v>
+      </c>
+      <c r="C9" t="s">
         <v>577</v>
-      </c>
-      <c r="C9" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
@@ -5177,18 +5177,18 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C11" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C12" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
   </sheetData>
@@ -5219,31 +5219,31 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>582</v>
+      </c>
+      <c r="C3" t="s">
         <v>583</v>
-      </c>
-      <c r="C3" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
   </sheetData>
@@ -5669,13 +5669,13 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -5708,7 +5708,7 @@
         <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>618</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -5738,10 +5738,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
         <v>118</v>
-      </c>
-      <c r="C6" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -5749,13 +5749,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" t="s">
         <v>120</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>121</v>
-      </c>
-      <c r="D7" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -5763,10 +5763,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
         <v>123</v>
-      </c>
-      <c r="C8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5774,10 +5774,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" t="s">
         <v>125</v>
-      </c>
-      <c r="C9" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -5785,10 +5785,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" t="s">
         <v>127</v>
-      </c>
-      <c r="C10" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5796,13 +5796,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" t="s">
         <v>129</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>130</v>
-      </c>
-      <c r="D11" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -5810,10 +5810,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" t="s">
         <v>132</v>
-      </c>
-      <c r="C12" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -5821,13 +5821,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" t="s">
         <v>134</v>
       </c>
-      <c r="C13" t="s">
-        <v>135</v>
-      </c>
       <c r="D13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -5835,13 +5835,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" t="s">
         <v>136</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>137</v>
-      </c>
-      <c r="D14" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -5849,13 +5849,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" t="s">
         <v>139</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>140</v>
-      </c>
-      <c r="D15" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -5863,10 +5863,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" t="s">
         <v>142</v>
-      </c>
-      <c r="C16" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -5874,13 +5874,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" t="s">
         <v>144</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>145</v>
-      </c>
-      <c r="D17" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -5888,10 +5888,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" t="s">
         <v>147</v>
-      </c>
-      <c r="C18" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -5899,10 +5899,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" t="s">
         <v>149</v>
-      </c>
-      <c r="C19" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -5910,10 +5910,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" t="s">
         <v>151</v>
-      </c>
-      <c r="C20" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -5921,10 +5921,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21" t="s">
         <v>153</v>
-      </c>
-      <c r="C21" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -5932,10 +5932,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" t="s">
         <v>155</v>
-      </c>
-      <c r="C22" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -5943,10 +5943,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" t="s">
         <v>157</v>
-      </c>
-      <c r="C23" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -5954,10 +5954,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" t="s">
         <v>159</v>
-      </c>
-      <c r="C24" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -5965,10 +5965,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" t="s">
         <v>161</v>
-      </c>
-      <c r="C25" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -5976,10 +5976,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -6051,13 +6051,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6065,10 +6065,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -6076,10 +6076,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -6087,10 +6087,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" t="s">
         <v>169</v>
-      </c>
-      <c r="C8" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6098,10 +6098,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" t="s">
         <v>171</v>
-      </c>
-      <c r="C9" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -6109,10 +6109,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" t="s">
         <v>173</v>
-      </c>
-      <c r="C10" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -6120,10 +6120,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C11" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6131,10 +6131,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" t="s">
         <v>176</v>
-      </c>
-      <c r="C12" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -6142,10 +6142,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" t="s">
         <v>178</v>
-      </c>
-      <c r="C13" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6153,10 +6153,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" t="s">
         <v>180</v>
-      </c>
-      <c r="C14" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -6167,7 +6167,7 @@
         <v>116</v>
       </c>
       <c r="C15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -6196,10 +6196,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" t="s">
         <v>184</v>
-      </c>
-      <c r="C2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -6207,10 +6207,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -6222,7 +6222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -6241,7 +6241,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6249,13 +6249,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" t="s">
         <v>188</v>
-      </c>
-      <c r="D2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6263,10 +6263,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -6274,10 +6274,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -6285,10 +6285,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C5" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6296,10 +6296,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>554</v>
+      </c>
+      <c r="C6" t="s">
         <v>555</v>
-      </c>
-      <c r="C6" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -6307,13 +6307,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C7" t="s">
+        <v>562</v>
+      </c>
+      <c r="D7" t="s">
         <v>563</v>
-      </c>
-      <c r="D7" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -6324,7 +6324,7 @@
         <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6332,10 +6332,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" t="s">
         <v>194</v>
-      </c>
-      <c r="C9" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -6343,10 +6343,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -6354,10 +6354,10 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
+        <v>196</v>
+      </c>
+      <c r="C11" t="s">
         <v>197</v>
-      </c>
-      <c r="C11" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6365,10 +6365,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -6376,10 +6376,10 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C13" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6387,19 +6387,19 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C14" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C15" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -6407,10 +6407,10 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
+        <v>200</v>
+      </c>
+      <c r="C16" t="s">
         <v>201</v>
-      </c>
-      <c r="C16" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -6418,10 +6418,10 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -6429,10 +6429,10 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C18" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -6440,10 +6440,10 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C19" t="s">
         <v>205</v>
-      </c>
-      <c r="C19" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -6451,10 +6451,10 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20" t="s">
         <v>207</v>
-      </c>
-      <c r="C20" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -6462,10 +6462,10 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C21" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -6473,10 +6473,10 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
+        <v>209</v>
+      </c>
+      <c r="C22" t="s">
         <v>210</v>
-      </c>
-      <c r="C22" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -6484,10 +6484,10 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C23" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -6495,10 +6495,10 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
+        <v>212</v>
+      </c>
+      <c r="C24" t="s">
         <v>213</v>
-      </c>
-      <c r="C24" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -6506,19 +6506,19 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" t="s">
+        <v>546</v>
+      </c>
+      <c r="C26" t="s">
         <v>547</v>
-      </c>
-      <c r="C26" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -6526,10 +6526,10 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
+        <v>217</v>
+      </c>
+      <c r="C27" t="s">
         <v>218</v>
-      </c>
-      <c r="C27" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -6537,10 +6537,10 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
+        <v>219</v>
+      </c>
+      <c r="C28" t="s">
         <v>220</v>
-      </c>
-      <c r="C28" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -6548,10 +6548,10 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C29" t="s">
         <v>222</v>
-      </c>
-      <c r="C29" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -6559,10 +6559,10 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
+        <v>223</v>
+      </c>
+      <c r="C30" t="s">
         <v>224</v>
-      </c>
-      <c r="C30" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -6570,10 +6570,10 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
+        <v>225</v>
+      </c>
+      <c r="C31" t="s">
         <v>226</v>
-      </c>
-      <c r="C31" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -6584,7 +6584,7 @@
         <v>47</v>
       </c>
       <c r="C32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -6592,10 +6592,10 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
+        <v>228</v>
+      </c>
+      <c r="C33" t="s">
         <v>229</v>
-      </c>
-      <c r="C33" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -6606,7 +6606,7 @@
         <v>66</v>
       </c>
       <c r="C34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -6614,10 +6614,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C35" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -6625,10 +6625,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
+        <v>233</v>
+      </c>
+      <c r="C36" t="s">
         <v>234</v>
-      </c>
-      <c r="C36" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -6636,10 +6636,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
+        <v>235</v>
+      </c>
+      <c r="C37" t="s">
         <v>236</v>
-      </c>
-      <c r="C37" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -6647,10 +6647,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C38" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -6658,10 +6658,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
+        <v>238</v>
+      </c>
+      <c r="C39" t="s">
         <v>239</v>
-      </c>
-      <c r="C39" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -6672,7 +6672,7 @@
         <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -6680,10 +6680,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C41" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -6691,10 +6691,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C42" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -6702,10 +6702,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>559</v>
+      </c>
+      <c r="C43" t="s">
         <v>560</v>
-      </c>
-      <c r="C43" t="s">
-        <v>561</v>
       </c>
     </row>
   </sheetData>
@@ -6737,7 +6737,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6745,10 +6745,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" t="s">
         <v>243</v>
-      </c>
-      <c r="C2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6756,10 +6756,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" t="s">
         <v>245</v>
-      </c>
-      <c r="C3" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -6767,10 +6767,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -6778,10 +6778,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C5" t="s">
         <v>248</v>
-      </c>
-      <c r="C5" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6789,10 +6789,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C6" t="s">
         <v>250</v>
-      </c>
-      <c r="C6" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -6800,10 +6800,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7" t="s">
         <v>252</v>
-      </c>
-      <c r="C7" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -6811,10 +6811,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C8" t="s">
         <v>254</v>
-      </c>
-      <c r="C8" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6822,10 +6822,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" t="s">
         <v>256</v>
-      </c>
-      <c r="C9" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -6833,10 +6833,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>257</v>
+      </c>
+      <c r="C10" t="s">
         <v>258</v>
-      </c>
-      <c r="C10" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -6844,10 +6844,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6855,10 +6855,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>260</v>
+      </c>
+      <c r="C12" t="s">
         <v>261</v>
-      </c>
-      <c r="C12" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -6866,10 +6866,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>262</v>
+      </c>
+      <c r="C13" t="s">
         <v>263</v>
-      </c>
-      <c r="C13" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6877,10 +6877,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C14" t="s">
         <v>265</v>
-      </c>
-      <c r="C14" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -6888,10 +6888,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>266</v>
+      </c>
+      <c r="C15" t="s">
         <v>267</v>
-      </c>
-      <c r="C15" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -6899,10 +6899,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>268</v>
+      </c>
+      <c r="C16" t="s">
         <v>269</v>
-      </c>
-      <c r="C16" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -6910,10 +6910,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>270</v>
+      </c>
+      <c r="C17" t="s">
         <v>271</v>
-      </c>
-      <c r="C17" t="s">
-        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Laden Airflow verbeterd ivm foutmeldingen
</commit_message>
<xml_diff>
--- a/data/wasstraat_config/Wasstraat_Config_HarmonizeV2.xlsx
+++ b/data/wasstraat_config/Wasstraat_Config_HarmonizeV2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Dropbox/Development/wasstraat_archeologische_data/data/wasstraat_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20ADB4B-973D-ED4A-9AC2-5E6012F8D3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D408138F-035B-FA47-98FD-A87B953F4CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Objecten" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
     <author>tc={EAE429C4-0AE8-B645-9B37-57AAB4AB828A}</author>
   </authors>
   <commentList>
-    <comment ref="B40" authorId="0" shapeId="0" xr:uid="{EAE429C4-0AE8-B645-9B37-57AAB4AB828A}">
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{EAE429C4-0AE8-B645-9B37-57AAB4AB828A}">
       <text>
         <t>[Opmerkingenthread]
 U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="617">
   <si>
     <t>Object</t>
   </si>
@@ -304,9 +304,6 @@
     <t>["BESCHRIJVING"]</t>
   </si>
   <si>
-    <t>datering</t>
-  </si>
-  <si>
     <t>["DAT", "DATERING"]</t>
   </si>
   <si>
@@ -589,9 +586,6 @@
     <t>["INHOUD", "OPMERKING"]</t>
   </si>
   <si>
-    <t>["VOORLOPIGEDATERING"]</t>
-  </si>
-  <si>
     <t>xcoor_rd</t>
   </si>
   <si>
@@ -682,12 +676,6 @@
     <t>['GECONSERVEERD', 'CONSERV', '14']</t>
   </si>
   <si>
-    <t>dateringtot</t>
-  </si>
-  <si>
-    <t>dateringvanaf</t>
-  </si>
-  <si>
     <t>diversen</t>
   </si>
   <si>
@@ -1912,27 +1900,12 @@
     <t>["VONDSTOMSTH", "VERZMWIJZE"]</t>
   </si>
   <si>
-    <t>voorlopige_datering</t>
-  </si>
-  <si>
     <t>['TOTAANTAL', 'AANTAL', '4b1']</t>
   </si>
   <si>
     <t>['COMPLEET', '6d', 'COMPL', 'FRAGM']</t>
   </si>
   <si>
-    <t>['DAT_CMPLX', 'DAT_COMPL', '1bcomplex']</t>
-  </si>
-  <si>
-    <t>['DAT_VRWP', 'OOR_DAT', 'DATERING', '3datering voorwerp', 'DATUM', '1c', '3']</t>
-  </si>
-  <si>
-    <t>datering_object</t>
-  </si>
-  <si>
-    <t>datering_complex</t>
-  </si>
-  <si>
     <t>['13', 'EXPO']</t>
   </si>
   <si>
@@ -1943,6 +1916,27 @@
   </si>
   <si>
     <t>["VULLING", "VULLINGNO", "MUUR"]</t>
+  </si>
+  <si>
+    <t>["VOORLOPIGEDATERING", "DAT", "DATERING"]</t>
+  </si>
+  <si>
+    <t>['DAT_VRWP', 'OOR_DAT', 'DATERING', '3datering voorwerp', 'DATUM', '1c', '3', 'DAT_CMPLX', 'DAT_COMPL']</t>
+  </si>
+  <si>
+    <t>artefactdatering</t>
+  </si>
+  <si>
+    <t>artefactdatering_tot</t>
+  </si>
+  <si>
+    <t>artefactdatering_vanaf</t>
+  </si>
+  <si>
+    <t>spoordatering</t>
+  </si>
+  <si>
+    <t>vondstdatering</t>
   </si>
 </sst>
 </file>
@@ -2362,7 +2356,7 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B40" dT="2022-05-04T13:22:53.89" personId="{2BE8FBFB-2E17-4B4E-BEE9-14B2389B829C}" id="{EAE429C4-0AE8-B645-9B37-57AAB4AB828A}">
+  <threadedComment ref="B39" dT="2022-05-04T13:22:53.89" personId="{2BE8FBFB-2E17-4B4E-BEE9-14B2389B829C}" id="{EAE429C4-0AE8-B645-9B37-57AAB4AB828A}">
     <text>Verplaatsen naar Vondst</text>
   </threadedComment>
 </ThreadedComments>
@@ -2399,7 +2393,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2484,10 +2478,10 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C9" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2495,10 +2489,10 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C10" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2548,7 +2542,7 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -2565,7 +2559,7 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2582,7 +2576,7 @@
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2599,7 +2593,7 @@
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -2616,7 +2610,7 @@
         <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -2627,13 +2621,13 @@
         <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>617</v>
+        <v>608</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -2650,7 +2644,7 @@
         <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -2661,13 +2655,13 @@
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -2675,7 +2669,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
@@ -2684,7 +2678,7 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -2692,16 +2686,16 @@
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="C23" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="D23" t="s">
         <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -2709,16 +2703,16 @@
         <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C24" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="D24" t="s">
         <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -2735,7 +2729,7 @@
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -2752,10 +2746,10 @@
         <v>20</v>
       </c>
       <c r="F26" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="G26" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -2772,7 +2766,7 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
   </sheetData>
@@ -2804,7 +2798,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2812,10 +2806,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2823,10 +2817,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2834,10 +2828,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2845,10 +2839,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2856,10 +2850,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2867,10 +2861,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C7" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2878,10 +2872,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C8" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2889,10 +2883,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C9" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -2923,7 +2917,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2931,10 +2925,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2942,10 +2936,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2953,10 +2947,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C4" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2964,10 +2958,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2975,10 +2969,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2986,10 +2980,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2997,10 +2991,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3008,10 +3002,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C9" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3019,10 +3013,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C10" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3030,10 +3024,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C11" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3041,10 +3035,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C12" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3052,10 +3046,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C13" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3063,10 +3057,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C14" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3074,10 +3068,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C15" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3085,10 +3079,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C16" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3096,10 +3090,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C17" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3107,10 +3101,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C18" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3118,10 +3112,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C19" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3129,10 +3123,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C20" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3140,10 +3134,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C21" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3151,10 +3145,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C22" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3162,10 +3156,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C23" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3173,10 +3167,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C24" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3184,10 +3178,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C25" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3195,10 +3189,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -3220,7 +3214,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>45</v>
@@ -3229,7 +3223,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3253,7 +3247,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3261,10 +3255,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3272,10 +3266,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3283,10 +3277,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C4" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3294,10 +3288,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C5" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3305,10 +3299,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3316,10 +3310,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3327,10 +3321,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C8" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3338,10 +3332,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C9" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3349,10 +3343,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C10" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3360,10 +3354,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C11" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -3387,7 +3381,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3413,7 +3407,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3421,10 +3415,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3432,10 +3426,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3443,10 +3437,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3454,10 +3448,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C5" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3465,10 +3459,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C6" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3476,10 +3470,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3487,10 +3481,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C8" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3498,10 +3492,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C9" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3509,10 +3503,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C10" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3520,10 +3514,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C11" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3531,10 +3525,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C12" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3542,10 +3536,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C13" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3553,10 +3547,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C14" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3564,10 +3558,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C15" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3575,10 +3569,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C16" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3586,10 +3580,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C17" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3597,10 +3591,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C18" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3608,10 +3602,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C19" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3619,10 +3613,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C20" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3630,10 +3624,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C21" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3641,10 +3635,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C22" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3652,10 +3646,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C23" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3663,10 +3657,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C24" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -3674,10 +3668,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C25" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3685,10 +3679,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C26" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3696,10 +3690,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C27" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3707,10 +3701,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C28" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3718,10 +3712,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C29" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -3729,10 +3723,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C30" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -3762,7 +3756,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3770,10 +3764,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C2" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3781,10 +3775,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C3" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3792,10 +3786,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C4" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3803,10 +3797,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C5" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3814,10 +3808,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C6" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3825,10 +3819,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C7" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3836,10 +3830,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3847,10 +3841,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C9" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3858,10 +3852,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C10" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3869,10 +3863,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C11" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3880,10 +3874,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C12" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3891,10 +3885,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C13" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3902,10 +3896,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C14" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3913,10 +3907,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C15" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3924,10 +3918,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C16" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3935,10 +3929,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C17" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3946,10 +3940,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C18" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3957,10 +3951,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C19" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3968,10 +3962,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C20" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3979,10 +3973,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C21" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3990,10 +3984,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C22" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -4001,10 +3995,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C23" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -4012,10 +4006,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C24" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -4023,10 +4017,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C25" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -4034,10 +4028,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C26" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -4045,10 +4039,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C27" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -4056,10 +4050,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -4087,7 +4081,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4095,10 +4089,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4106,10 +4100,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C3" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4117,10 +4111,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C4" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4128,10 +4122,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C5" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4139,10 +4133,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4150,10 +4144,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C7" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4161,10 +4155,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C8" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4172,10 +4166,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C9" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4183,10 +4177,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C10" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4194,10 +4188,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4205,10 +4199,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C12" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4216,10 +4210,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C13" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4227,10 +4221,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C14" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4238,10 +4232,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C15" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4249,10 +4243,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="C16" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -4260,10 +4254,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C17" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -4271,10 +4265,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C18" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -4298,7 +4292,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4306,10 +4300,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C2" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4317,10 +4311,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C3" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4328,10 +4322,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4339,10 +4333,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4350,10 +4344,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C6" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4361,10 +4355,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C7" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4372,10 +4366,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C8" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4383,10 +4377,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C9" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4394,10 +4388,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C10" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4405,10 +4399,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C11" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4416,10 +4410,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C12" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4427,10 +4421,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C13" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4438,10 +4432,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C14" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4449,10 +4443,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C15" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4460,10 +4454,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C16" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -4471,10 +4465,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C17" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -4498,7 +4492,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4506,10 +4500,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4517,10 +4511,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C3" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4528,10 +4522,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C4" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4539,10 +4533,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C5" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4550,10 +4544,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C6" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4561,10 +4555,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C7" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4572,10 +4566,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C8" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4583,10 +4577,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C9" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4594,10 +4588,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C10" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4605,10 +4599,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C11" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4616,10 +4610,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4627,10 +4621,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C13" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4638,10 +4632,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="C14" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4649,10 +4643,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C15" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4660,10 +4654,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C16" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -4671,10 +4665,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C17" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -4682,10 +4676,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C18" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -4693,10 +4687,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C19" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -4704,10 +4698,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="C20" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -4715,10 +4709,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="C21" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -4726,10 +4720,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="C22" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -4737,10 +4731,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C23" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -4748,10 +4742,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C24" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -4759,10 +4753,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -4770,10 +4764,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="C26" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>
@@ -4883,7 +4877,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4891,10 +4885,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="C2" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4902,10 +4896,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C3" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4913,10 +4907,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C4" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4924,10 +4918,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="C5" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4935,10 +4929,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C6" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4946,10 +4940,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C7" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4957,10 +4951,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C8" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4968,10 +4962,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C9" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4979,10 +4973,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C10" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4990,10 +4984,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C11" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -5001,10 +4995,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="C12" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -5012,10 +5006,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C13" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -5023,10 +5017,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="C14" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -5034,10 +5028,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C15" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -5045,10 +5039,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C16" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -5056,10 +5050,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C17" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -5067,10 +5061,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C18" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -5100,31 +5094,31 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C2" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C4" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
@@ -5140,7 +5134,7 @@
         <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
@@ -5148,47 +5142,47 @@
         <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="C9" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" t="s">
         <v>106</v>
-      </c>
-      <c r="C10" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C11" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C12" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
   </sheetData>
@@ -5219,31 +5213,31 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C2" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="C3" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C4" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
   </sheetData>
@@ -5340,7 +5334,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView zoomScale="240" zoomScaleNormal="240" workbookViewId="0"/>
+    <sheetView zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5423,10 +5419,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C7" t="s">
         <v>72</v>
-      </c>
-      <c r="C7" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -5434,10 +5430,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
         <v>74</v>
-      </c>
-      <c r="C8" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5445,10 +5441,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
         <v>76</v>
-      </c>
-      <c r="C9" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -5456,10 +5452,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
         <v>78</v>
-      </c>
-      <c r="C10" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5467,10 +5463,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" t="s">
         <v>80</v>
-      </c>
-      <c r="C11" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -5478,10 +5474,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" t="s">
         <v>82</v>
-      </c>
-      <c r="C12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -5489,10 +5485,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
         <v>84</v>
-      </c>
-      <c r="C13" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -5500,10 +5496,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" t="s">
         <v>86</v>
-      </c>
-      <c r="C14" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -5511,10 +5507,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" t="s">
         <v>88</v>
-      </c>
-      <c r="C15" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -5522,13 +5518,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
         <v>90</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>91</v>
-      </c>
-      <c r="D16" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -5536,10 +5532,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" t="s">
         <v>93</v>
-      </c>
-      <c r="C17" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -5547,13 +5543,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" t="s">
         <v>95</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>96</v>
-      </c>
-      <c r="D18" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -5561,13 +5557,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" t="s">
         <v>98</v>
       </c>
-      <c r="C19" t="s">
-        <v>99</v>
-      </c>
       <c r="D19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -5575,13 +5571,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" t="s">
         <v>100</v>
       </c>
-      <c r="C20" t="s">
-        <v>101</v>
-      </c>
       <c r="D20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -5589,13 +5585,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" t="s">
         <v>102</v>
       </c>
-      <c r="C21" t="s">
-        <v>103</v>
-      </c>
       <c r="D21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -5603,10 +5599,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" t="s">
         <v>104</v>
-      </c>
-      <c r="C22" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -5614,10 +5610,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" t="s">
         <v>106</v>
-      </c>
-      <c r="C23" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -5625,10 +5621,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" t="s">
         <v>108</v>
-      </c>
-      <c r="C24" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -5636,13 +5632,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" t="s">
         <v>110</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>111</v>
-      </c>
-      <c r="D25" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -5650,13 +5646,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" t="s">
         <v>113</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>114</v>
-      </c>
-      <c r="D26" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -5668,7 +5664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -5705,10 +5701,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>618</v>
+        <v>609</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -5738,10 +5734,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" t="s">
         <v>117</v>
-      </c>
-      <c r="C6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -5749,13 +5745,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" t="s">
         <v>119</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>120</v>
-      </c>
-      <c r="D7" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -5763,10 +5759,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" t="s">
         <v>122</v>
-      </c>
-      <c r="C8" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5774,10 +5770,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
         <v>124</v>
-      </c>
-      <c r="C9" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -5785,10 +5781,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" t="s">
         <v>126</v>
-      </c>
-      <c r="C10" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5796,13 +5792,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" t="s">
         <v>128</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>129</v>
-      </c>
-      <c r="D11" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -5810,10 +5806,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" t="s">
         <v>131</v>
-      </c>
-      <c r="C12" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -5821,13 +5817,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" t="s">
         <v>133</v>
       </c>
-      <c r="C13" t="s">
-        <v>134</v>
-      </c>
       <c r="D13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -5835,13 +5831,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" t="s">
         <v>135</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>136</v>
-      </c>
-      <c r="D14" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -5849,13 +5845,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" t="s">
         <v>138</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>139</v>
-      </c>
-      <c r="D15" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -5863,10 +5859,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" t="s">
         <v>141</v>
-      </c>
-      <c r="C16" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -5874,13 +5870,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" t="s">
         <v>143</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>144</v>
-      </c>
-      <c r="D17" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -5888,10 +5884,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" t="s">
         <v>146</v>
-      </c>
-      <c r="C18" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -5899,10 +5895,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" t="s">
         <v>148</v>
-      </c>
-      <c r="C19" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -5910,10 +5906,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" t="s">
         <v>150</v>
-      </c>
-      <c r="C20" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -5921,10 +5917,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" t="s">
         <v>152</v>
-      </c>
-      <c r="C21" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -5932,10 +5928,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" t="s">
         <v>154</v>
-      </c>
-      <c r="C22" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -5943,10 +5939,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" t="s">
         <v>156</v>
-      </c>
-      <c r="C23" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -5954,10 +5950,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" t="s">
         <v>158</v>
-      </c>
-      <c r="C24" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -5965,10 +5961,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" t="s">
         <v>160</v>
-      </c>
-      <c r="C25" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -5976,10 +5972,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -5991,14 +5987,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6051,13 +6047,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C5" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="D5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6065,10 +6061,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -6076,10 +6072,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>608</v>
+        <v>616</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>610</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -6087,10 +6083,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6098,10 +6094,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -6109,10 +6105,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -6120,10 +6116,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C11" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6131,10 +6127,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -6142,10 +6138,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6153,10 +6149,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -6164,10 +6160,10 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -6196,10 +6192,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -6207,10 +6203,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -6220,10 +6216,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6241,7 +6237,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6249,13 +6245,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="C2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6263,10 +6259,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -6274,10 +6270,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -6285,10 +6281,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C5" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6296,10 +6292,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C6" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -6307,13 +6303,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C7" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D7" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -6324,7 +6320,7 @@
         <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6332,10 +6328,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -6343,10 +6339,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C10" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -6354,10 +6350,10 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6365,10 +6361,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -6376,10 +6372,10 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>198</v>
+        <v>613</v>
       </c>
       <c r="C13" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6387,325 +6383,316 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>199</v>
+        <v>614</v>
       </c>
       <c r="C14" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="3" t="s">
-        <v>614</v>
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>196</v>
       </c>
       <c r="C15" t="s">
-        <v>611</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="C16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="C17" t="s">
-        <v>202</v>
+        <v>606</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C18" t="s">
-        <v>615</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C20" t="s">
-        <v>207</v>
+        <v>544</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C21" t="s">
-        <v>548</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C22" t="s">
-        <v>210</v>
+        <v>554</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C23" t="s">
-        <v>558</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>212</v>
+        <v>541</v>
       </c>
       <c r="C24" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" t="s">
+        <v>542</v>
+      </c>
+      <c r="C25" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>545</v>
-      </c>
-      <c r="C25" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" t="s">
-        <v>546</v>
-      </c>
       <c r="C26" t="s">
-        <v>547</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C27" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C29" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C30" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>225</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>224</v>
       </c>
       <c r="C32" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>228</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>228</v>
       </c>
       <c r="C34" t="s">
-        <v>231</v>
+        <v>557</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C35" t="s">
-        <v>561</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C36" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C37" t="s">
-        <v>236</v>
+        <v>548</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C38" t="s">
-        <v>552</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>238</v>
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>38</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>58</v>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>172</v>
       </c>
       <c r="C40" t="s">
-        <v>240</v>
+        <v>537</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>174</v>
+        <v>607</v>
       </c>
       <c r="C41" t="s">
-        <v>541</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <v>41</v>
+      <c r="A42" s="2">
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>616</v>
+        <v>555</v>
       </c>
       <c r="C42" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>559</v>
-      </c>
-      <c r="C43" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
   </sheetData>
@@ -6737,7 +6724,7 @@
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6745,10 +6732,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6756,10 +6743,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -6767,10 +6754,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -6778,10 +6765,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6789,10 +6776,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C6" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -6800,10 +6787,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C7" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -6811,10 +6798,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C8" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6822,10 +6809,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C9" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -6833,10 +6820,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C10" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -6844,10 +6831,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C11" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6855,10 +6842,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C12" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -6866,10 +6853,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C13" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6877,10 +6864,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C14" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -6888,10 +6875,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C15" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -6899,10 +6886,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C16" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -6910,10 +6897,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C17" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>